<commit_message>
diagram + grammar is done
</commit_message>
<xml_diff>
--- a/alng.xlsx
+++ b/alng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Desktop\NURE\Semestr2\AOTI(avtomatichna_obrobka_tekstovoii_informatsii)\aoti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D6D8A8-7877-4F1B-BE3B-C4B9E5D0DC47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B8F950-03A1-48B1-82F9-15910A61C6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="75">
   <si>
     <t>cond</t>
   </si>
@@ -42,9 +42,6 @@
     <t>}</t>
   </si>
   <si>
-    <t>(</t>
-  </si>
-  <si>
     <t>)</t>
   </si>
   <si>
@@ -66,24 +63,12 @@
     <t>eq, less, greater, less_eq, greater_eq</t>
   </si>
   <si>
-    <t>comparison</t>
-  </si>
-  <si>
     <t>false, true</t>
   </si>
   <si>
     <t>boolean</t>
   </si>
   <si>
-    <t>arithmetical</t>
-  </si>
-  <si>
-    <t>plu, min, mul, div, inc</t>
-  </si>
-  <si>
-    <t>cycle</t>
-  </si>
-  <si>
     <t>atomical -&gt; number | boolean | identifier | array_access</t>
   </si>
   <si>
@@ -115,6 +100,156 @@
   </si>
   <si>
     <t>comparison -&gt; arithmetic comparison_operator comparison | arithmetic</t>
+  </si>
+  <si>
+    <t>plu, min, mul, div</t>
+  </si>
+  <si>
+    <t>inc dec</t>
+  </si>
+  <si>
+    <t>cycle(</t>
+  </si>
+  <si>
+    <t>comparison stmt_body</t>
+  </si>
+  <si>
+    <t>stmt_body = stmt_inc</t>
+  </si>
+  <si>
+    <t>assignment</t>
+  </si>
+  <si>
+    <t>result_stmt assignable</t>
+  </si>
+  <si>
+    <t>assignable</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable </t>
+  </si>
+  <si>
+    <t>variable{variable_as_index}</t>
+  </si>
+  <si>
+    <t>variable_as_index</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>arithmetic_binary_op</t>
+  </si>
+  <si>
+    <t>arithmetic_unary_op</t>
+  </si>
+  <si>
+    <t>comparison_binary_op</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unary_op </t>
+  </si>
+  <si>
+    <t>unary_op</t>
+  </si>
+  <si>
+    <t>unary_op variable non_empty_result_stmt</t>
+  </si>
+  <si>
+    <t>For example:</t>
+  </si>
+  <si>
+    <t>ROOT</t>
+  </si>
+  <si>
+    <t>STMT</t>
+  </si>
+  <si>
+    <t>COMPARISON</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT</t>
+  </si>
+  <si>
+    <t>ASSIGNABLE</t>
+  </si>
+  <si>
+    <t>VARIABLE</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>NE_RES_STMT</t>
+  </si>
+  <si>
+    <t>RES_STMT</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT COMPARISON STMT STMT</t>
+  </si>
+  <si>
+    <t>ASSIGNABLE RES_STMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NE_RES_STMT</t>
+  </si>
+  <si>
+    <t>assignment res_stmt stmt_body stmt_inc</t>
+  </si>
+  <si>
+    <t>res_stmt</t>
+  </si>
+  <si>
+    <t>ne_res_stmt</t>
+  </si>
+  <si>
+    <t>variable ne_res_stmt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value ne_res_stmt</t>
+  </si>
+  <si>
+    <t>BINARY_OP</t>
+  </si>
+  <si>
+    <t>binary_op</t>
+  </si>
+  <si>
+    <t>operator variable</t>
+  </si>
+  <si>
+    <t>operator value</t>
+  </si>
+  <si>
+    <t>OPERATOR</t>
+  </si>
+  <si>
+    <t>binary_op ne_res_stmt</t>
+  </si>
+  <si>
+    <t>NE_RES_RESULT</t>
+  </si>
+  <si>
+    <t>stmt</t>
+  </si>
+  <si>
+    <t>stmt stmt</t>
+  </si>
+  <si>
+    <t>UNARY_OP</t>
+  </si>
+  <si>
+    <t>e stmt</t>
+  </si>
+  <si>
+    <t>assignment stmt</t>
+  </si>
+  <si>
+    <t>value ne_res_stmt</t>
   </si>
 </sst>
 </file>
@@ -432,131 +567,570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:U11"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.90625" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="10" max="10" width="30.81640625" customWidth="1"/>
+    <col min="3" max="3" width="41.36328125" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" customWidth="1"/>
+    <col min="9" max="9" width="6.90625" customWidth="1"/>
+    <col min="10" max="10" width="9.6328125" customWidth="1"/>
     <col min="11" max="11" width="10.26953125" customWidth="1"/>
     <col min="12" max="12" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>3</v>
       </c>
-      <c r="N5" t="s">
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="O5" t="s">
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="P5" t="s">
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="R5" t="s">
+      <c r="F28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>8</v>
       </c>
-      <c r="S5" t="s">
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="T5" t="s">
+      <c r="F30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
         <v>10</v>
       </c>
-      <c r="U5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>20</v>
+      <c r="H31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" t="s">
+        <v>74</v>
+      </c>
+      <c r="K31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" t="s">
+        <v>45</v>
+      </c>
+      <c r="K39" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" t="s">
+        <v>45</v>
+      </c>
+      <c r="M39" t="s">
+        <v>45</v>
+      </c>
+      <c r="N39" t="s">
+        <v>45</v>
+      </c>
+      <c r="O39" t="s">
+        <v>45</v>
+      </c>
+      <c r="P39" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" t="s">
+        <v>46</v>
+      </c>
+      <c r="K40" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" t="s">
+        <v>46</v>
+      </c>
+      <c r="M40" t="s">
+        <v>46</v>
+      </c>
+      <c r="N40" t="s">
+        <v>46</v>
+      </c>
+      <c r="O40" t="s">
+        <v>46</v>
+      </c>
+      <c r="P40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" t="s">
+        <v>46</v>
+      </c>
+      <c r="K41" t="s">
+        <v>46</v>
+      </c>
+      <c r="L41" t="s">
+        <v>46</v>
+      </c>
+      <c r="M41" t="s">
+        <v>46</v>
+      </c>
+      <c r="N41" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" t="s">
+        <v>46</v>
+      </c>
+      <c r="P41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" t="s">
+        <v>47</v>
+      </c>
+      <c r="I42" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" t="s">
+        <v>52</v>
+      </c>
+      <c r="K42" t="s">
+        <v>52</v>
+      </c>
+      <c r="L42" t="s">
+        <v>52</v>
+      </c>
+      <c r="M42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N42" t="s">
+        <v>52</v>
+      </c>
+      <c r="O42" t="s">
+        <v>62</v>
+      </c>
+      <c r="P42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" t="s">
+        <v>50</v>
+      </c>
+      <c r="K43" t="s">
+        <v>62</v>
+      </c>
+      <c r="L43" t="s">
+        <v>66</v>
+      </c>
+      <c r="M43" t="s">
+        <v>66</v>
+      </c>
+      <c r="O43" t="s">
+        <v>68</v>
+      </c>
+      <c r="P43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" t="s">
+        <v>51</v>
+      </c>
+      <c r="L44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RULES ARE IN DRAFT
</commit_message>
<xml_diff>
--- a/alng.xlsx
+++ b/alng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Desktop\NURE\Semestr2\AOTI(avtomatichna_obrobka_tekstovoii_informatsii)\aoti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B8F950-03A1-48B1-82F9-15910A61C6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A369952-51A9-4A7B-9D6A-5A008B1A413E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,12 +265,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,8 +291,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,20 +577,20 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.90625" customWidth="1"/>
-    <col min="3" max="3" width="41.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" customWidth="1"/>
+    <col min="4" max="4" width="4.1796875" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7265625" customWidth="1"/>
-    <col min="9" max="9" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" customWidth="1"/>
+    <col min="9" max="9" width="24.26953125" customWidth="1"/>
     <col min="10" max="10" width="9.6328125" customWidth="1"/>
     <col min="11" max="11" width="10.26953125" customWidth="1"/>
     <col min="12" max="12" width="13.26953125" customWidth="1"/>
@@ -653,7 +660,7 @@
       <c r="C15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E15" t="s">
@@ -685,6 +692,7 @@
       <c r="C16" t="s">
         <v>57</v>
       </c>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -693,6 +701,7 @@
       <c r="C17" t="s">
         <v>28</v>
       </c>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
@@ -701,6 +710,7 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -709,6 +719,7 @@
       <c r="C19" t="s">
         <v>37</v>
       </c>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -717,6 +728,7 @@
       <c r="B20" t="s">
         <v>40</v>
       </c>
+      <c r="D20" s="1"/>
       <c r="I20" t="s">
         <v>67</v>
       </c>
@@ -728,6 +740,7 @@
       <c r="B21" t="s">
         <v>13</v>
       </c>
+      <c r="D21" s="1"/>
       <c r="H21" t="s">
         <v>61</v>
       </c>
@@ -742,6 +755,7 @@
       <c r="B22" t="s">
         <v>38</v>
       </c>
+      <c r="D22" s="1"/>
       <c r="I22" t="s">
         <v>67</v>
       </c>
@@ -756,6 +770,7 @@
       <c r="C23" t="s">
         <v>41</v>
       </c>
+      <c r="D23" s="1"/>
       <c r="H23" t="s">
         <v>41</v>
       </c>
@@ -764,6 +779,7 @@
       <c r="B24" t="s">
         <v>3</v>
       </c>
+      <c r="D24" s="1"/>
       <c r="F24" t="s">
         <v>35</v>
       </c>
@@ -772,6 +788,7 @@
       <c r="B25" t="s">
         <v>4</v>
       </c>
+      <c r="D25" s="1"/>
       <c r="F25" t="s">
         <v>37</v>
       </c>
@@ -783,6 +800,7 @@
       <c r="B26" t="s">
         <v>5</v>
       </c>
+      <c r="D26" s="1"/>
       <c r="F26" t="s">
         <v>37</v>
       </c>
@@ -797,6 +815,7 @@
       <c r="C27" t="s">
         <v>69</v>
       </c>
+      <c r="D27" s="1"/>
       <c r="F27" t="s">
         <v>72</v>
       </c>
@@ -811,6 +830,7 @@
       <c r="B28" t="s">
         <v>7</v>
       </c>
+      <c r="D28" s="1"/>
       <c r="F28" t="s">
         <v>37</v>
       </c>
@@ -825,7 +845,7 @@
       <c r="C29" t="s">
         <v>73</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E29" t="s">

</xml_diff>